<commit_message>
Modifiche minori su selezione metriche e interazione utente
Modifiche per la visualizzazione del dataset e delle features in fase iniziale (preprocessing), dove utente visualizza le modifiche apportate al dataset e alle features durante gestione dei NaN e scaling.
Aggiunta la selezione delle metriche da parte dell'utente per i plot e le metriche salvate in file .xlsx.
Modifiche minori nei print per l'utente (aggiunta di mappatura della selezione del metodo di validazione da parte dell'utente, per printare il metodo scelto).
</commit_message>
<xml_diff>
--- a/model_performance.xlsx
+++ b/model_performance.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9587719298245614</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.0412280701754386</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9655629139072848</v>
+        <v>0.9655172413793104</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9454545454545454</v>
+        <v>0.9484536082474226</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9554558314626471</v>
+        <v>0.9569473921858529</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9555070095467447</v>
+        <v>0.9636889949723224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modifiche ai test metodi di validazione e aggiornato requirements.txt
Modificati i test dei metodi di validazione, in particolare il test sul metodo evaluate, in quanto l'output del metodo è stato modificato nei precedenti commit.
Specificato l'engine con cui le metriche vengono salvate nel file .xlsx e aggiornato requirements.txt con openpyxl.
</commit_message>
<xml_diff>
--- a/model_performance.xlsx
+++ b/model_performance.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.96</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9655172413793104</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9484536082474226</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9569473921858529</v>
+        <v>0.9595311355031686</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9636889949723224</v>
+        <v>0.9686</v>
       </c>
     </row>
   </sheetData>

</xml_diff>